<commit_message>
Interpolated NH4 permeability for pH 4.5 and 7
</commit_message>
<xml_diff>
--- a/Wastewater_Effluent_Filtration/BW30LE_pH4.5.xlsx
+++ b/Wastewater_Effluent_Filtration/BW30LE_pH4.5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mangu\Desktop\Nir Water Lab\High-Recovery-Effluent-RO\Wastewater_Effluent_Filtration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F793506-1827-4AA8-9059-D3A5E9B36F7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A9DADA0-DF04-44F0-8A9A-54C954107082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2149,6 +2149,7 @@
         <c:axId val="418944704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="4"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2290,7 +2291,2181 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Feed</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> pH 4.5</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-IL"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-IL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Brine pH</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$96</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="95"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>94</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$L$2:$L$96</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="95"/>
+                <c:pt idx="0">
+                  <c:v>4.5000274140699412</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.502735499236981</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.5054913850091562</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.5082846064270639</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.5111160847105669</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.5139871930309461</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.5168984116064017</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.5198503817090261</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.5228441120613221</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.5258807282755029</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.5289608471113656</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.5320857558861913</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.5352561457937766</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.5384731650137571</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.54173800301791</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.5450513174534404</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.5484145672354988</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.5518290410319064</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.5552956688751802</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.5588158098190759</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4.5623906118222672</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4.5660212674345511</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4.569709643282903</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4.5734565938461964</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4.5772638665517116</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4.581133118675166</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4.5850654749281468</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>4.5890629532309468</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4.5931268991679346</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>4.5972596543575417</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4.6014621138459777</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>4.605737021641426</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4.6100857820505352</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>4.6145105961216242</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>4.6190138225957842</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>4.6235973082960697</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>4.6282632832766799</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>4.633014541053055</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>4.6378530963176656</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>4.642781725425654</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4.6478032343018496</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>4.6529204087171481</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>4.6581362090449492</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>4.6634535324942963</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>4.6688756266001761</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>4.6744062895445477</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4.6800507883938343</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>4.6859211559681224</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>4.691908960555093</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>4.6980240896431704</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>4.7042707045324974</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>4.7106536176082718</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>4.717178023849244</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>4.7238492466135371</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>4.7306721570221981</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>4.7376534115846267</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>4.7447986837591936</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>4.7521146482326406</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>4.7596084368184748</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>4.767287359076219</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>4.7751591031348486</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>4.7832317313015196</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>4.7915148710868456</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>4.8000172377277597</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>4.8087495961677886</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>4.8177221880358214</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>4.8269467369859411</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>4.8364359111795032</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>4.8462029171675471</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>4.8562616950347097</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>4.8666280078603474</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>4.8773201314981991</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>4.8884820824267514</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>4.9000066847812658</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>4.911923007899583</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>4.9242549022295394</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>4.9370283106663013</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>4.9502713323280032</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>4.9640143665380139</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>4.9782904731575286</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>4.9931353197824384</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>5.0085873974763517</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>5.0246878797561054</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>5.0414799122019582</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>5.0590075890237536</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>5.0773153857774922</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>5.0964586310775353</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>5.1187744125213879</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>5.1420977062175401</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>5.1668296137700764</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>5.1930954812655603</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>5.2210124338560204</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>5.2506512172260171</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>5.2819496459373587</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>5.3144950788353036</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-770B-4EAA-AFE6-1925DB4FA651}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Permeate pH</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$96</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="95"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>94</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$M$2:$M$96</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="95"/>
+                <c:pt idx="0">
+                  <c:v>4.137207162893116</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.1358661995443464</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.1363474657765398</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.1368245227140452</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.1373112298305914</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.137815024292637</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.1383305494449329</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.1388583367568117</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.1393994458167711</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.1399551127666969</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.1405261454320588</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.1411138984695741</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.1417161593204126</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.1423338171888027</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.1429721912150148</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.1436253045714038</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.1442981940238974</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.1449924313033151</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.1457062144094747</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.1464411834698733</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4.1471990694025989</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4.1479783748888872</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4.1487842933849919</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4.149612368852754</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4.1504677899760027</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4.1513532931690831</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4.1522641251642014</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>4.1532063588208548</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4.1541792966881737</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>4.1551894609870317</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4.1562292253681123</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>4.1573091825029733</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4.1584252754535438</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>4.1595814907875939</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>4.1607819785232207</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>4.1620271225031367</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>4.1633176514558201</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>4.1646587527586707</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>4.1660516957891094</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>4.1674985102415398</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4.1690047316521586</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>4.1705734640936862</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>4.1722078703024748</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>4.1739111395022057</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>4.1756875299308138</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>4.1775460289582886</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4.1651101446122336</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>4.1675904739503817</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>4.1693977935285904</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>4.1712992689526498</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>4.1732901721158644</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>4.175387839096925</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>4.1775843042147676</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>4.1798965405577766</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>4.1823265606771498</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>4.1848911328742631</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>4.187595473361438</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>4.1904536916658888</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>4.1934781729288302</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>4.1966836030302659</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>4.2000843707707158</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>4.2036937051221601</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>4.2075394830517716</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>4.2116354011494739</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>4.2160140072992869</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>4.2206953934436386</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>4.2257121990723796</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>4.2311050407395836</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>4.2369107728079447</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>4.2431729223266528</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>4.2499492260886642</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>4.2441443461488397</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>4.2523865574423692</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>4.2604508686004676</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>4.2692802992000276</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>4.2790017323982923</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>4.2896886502543019</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>4.3015160927400551</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>4.3146582247982188</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>4.3293290104472861</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>4.3457842214411606</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>4.3643383507199633</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>4.3853762048473133</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>4.4093630715428436</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>4.43687611822169</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>4.4686104293224238</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>4.3378769645458961</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>4.388857289453556</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>4.4212469550872484</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>4.4601620218508806</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>4.5073164547951263</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>4.5654608802743786</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>4.6386982928500986</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>4.7331277648859693</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>4.8556349235715039</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-770B-4EAA-AFE6-1925DB4FA651}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$N$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Film layer pH</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$96</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="95"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>94</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$N$2:$N$96</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="95"/>
+                <c:pt idx="0">
+                  <c:v>4.5301272751534549</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.5267892843731596</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.5299095616452139</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.5330153183637121</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.5361438381950387</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.5393623696526824</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.542614323090743</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.5459044856389959</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.549238403711982</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.55262275616953</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.5560623201320798</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.5595640591042352</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.5631040115818626</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.5666888934235654</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.5703547946862484</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.574050747957747</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.577812801576254</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.5816483792503506</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.5855373948081768</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.5894879389738881</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4.5935084333509364</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4.5975795058131386</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4.6017385193921774</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4.6059402626456469</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4.6102219770642954</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4.6145938009180512</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4.6190135487991233</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>4.6235187626740428</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4.6280948867528959</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>4.6327808722274906</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4.6375116042608173</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>4.6423521556233727</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4.6472657268245028</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>4.6522673630817</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>4.6573725619729567</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>4.662572406264168</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>4.6678596633136964</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>4.6732527369115822</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>4.6787459156012918</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>4.6843359689066384</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4.69004284758865</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>4.6958655586752238</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>4.7018044038948927</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>4.7078606865555432</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>4.7140377098705759</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>4.7203623645039299</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4.7195536935764419</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>4.7262212318241863</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>4.7329294838182756</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>4.7398073850362286</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>4.7468220866692583</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>4.7539898135521836</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>4.7613367246026836</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>4.7688655780792111</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>4.7765482464023474</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>4.7844341370543821</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>4.7925031861768996</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>4.8007761367126527</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>4.8092613889370153</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>4.8179717092517791</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>4.8269093459698844</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>4.8360670735552569</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>4.8454934412125574</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>4.8551643259014883</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>4.8651274638729429</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>4.8753636883366456</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>4.8858949453552221</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>4.8967548304337054</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>4.907947712598709</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>4.9194800249367514</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>4.9313874054185103</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>4.935349925741515</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>4.9479866737831211</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>4.9611346990313763</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>4.9747555414126587</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>4.9888751478182236</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>5.0035485781169156</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>5.0188038509562256</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>5.0346793439470732</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>5.0512257468297808</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>5.068489546475754</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>5.0865326430865938</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>5.1054236351523059</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>5.1252290243917296</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>5.1460380937237673</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>5.1679402050816368</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>5.2006776651087332</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>5.2245370883492139</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>5.2527664522145354</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>5.2831358038387632</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>5.3157377888302548</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>5.3508792640595741</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>5.3889417804737469</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>5.4304308642893746</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>5.4761946471212557</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-770B-4EAA-AFE6-1925DB4FA651}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="407118192"/>
+        <c:axId val="418944704"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="407118192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-IL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="418944704"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="418944704"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="4"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-IL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="407118192"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-IL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-IL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -2846,20 +5021,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>15874</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:colOff>34924</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>546099</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>146050</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2879,6 +5570,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>15874</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>120650</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D43CB62-5B36-63E6-C64F-4E2913B094F4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3177,7 +5904,7 @@
   <dimension ref="A1:X96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7380,7 +10107,7 @@
         <v>7.1722049217775308E-3</v>
       </c>
       <c r="E67">
-        <f t="shared" ref="E67:E97" si="1">1-(D67/C67)</f>
+        <f t="shared" ref="E67:E96" si="1">1-(D67/C67)</f>
         <v>0.92691003874641476</v>
       </c>
       <c r="F67">

</xml_diff>